<commit_message>
pushing spec to README
</commit_message>
<xml_diff>
--- a/example/eO/data/demo-model.xlsx
+++ b/example/eO/data/demo-model.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/desho/CORAL-eO/example/eO/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86FE5571-5A21-FF4D-B192-52A8665D3ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4E9555-426C-A940-AF4B-049721BBE8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6020" yWindow="-16940" windowWidth="27300" windowHeight="16940" xr2:uid="{41EA2DF5-8191-DF45-B22C-AF15C792A506}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="27300" windowHeight="16940" xr2:uid="{41EA2DF5-8191-DF45-B22C-AF15C792A506}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="10000" iterateDelta="1E-14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,26 +34,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
-  <si>
-    <t>** CropReactor</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Area</t>
-  </si>
-  <si>
     <t>LettuceReactor</t>
   </si>
   <si>
     <t>Hab</t>
   </si>
   <si>
-    <t>Lettuce</t>
-  </si>
-  <si>
     <t>Temperature</t>
   </si>
   <si>
@@ -78,12 +69,6 @@
     <t>Contains</t>
   </si>
   <si>
-    <t>Inside</t>
-  </si>
-  <si>
-    <t>** Habitat Modules</t>
-  </si>
-  <si>
     <t>0.05/24</t>
   </si>
   <si>
@@ -94,6 +79,42 @@
   </si>
   <si>
     <t>/Users/desho/echusOverlook/Simulation/MarsOne/bean_test.xlsx</t>
+  </si>
+  <si>
+    <t>** Crew</t>
+  </si>
+  <si>
+    <t>** Habitat</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>Within</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>astro1</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>astro2</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -445,135 +466,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7E728F-F7B2-9840-B2B6-5DB10E2231F1}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B3">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>15</v>
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3">
+        <v>1.7649999999999999</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <v>55</v>
+      </c>
+      <c r="D4">
+        <v>1.63</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
         <v>70.3</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>25000</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>1E-3</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>0.73399999999999999</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>17</v>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>